<commit_message>
WIP: migration script completed
</commit_message>
<xml_diff>
--- a/cms/metrics_documentation/migration_data/metrics_definitions_migration.xlsx
+++ b/cms/metrics_documentation/migration_data/metrics_definitions_migration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipstanley/Documents/projects/UKHSA/winter-pressures/winter-pressures-api/cms/metrics_documentation/migration_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0990A454-ED2E-444A-B452-F053B05510CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C941D63-5239-BA46-995D-3DB7602D196E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="600" windowWidth="37220" windowHeight="22140" xr2:uid="{761B9231-95BC-4CC1-BF4F-419CF0B37169}"/>
+    <workbookView xWindow="800" yWindow="620" windowWidth="20800" windowHeight="27320" xr2:uid="{761B9231-95BC-4CC1-BF4F-419CF0B37169}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="234">
   <si>
     <t>Virus</t>
   </si>
@@ -158,9 +158,6 @@
 A change from a number greater than 0 to 0 will be displayed as -100% i.e. a 100% decrease</t>
   </si>
   <si>
-    <t>COVID-10_cases_casesByDay</t>
-  </si>
-  <si>
     <t xml:space="preserve">This metric shows the number of reported new cases for each day. 
 New cases are reported by specimen date - the date the first sample that identified the infection was taken from an individual.
 </t>
@@ -178,9 +175,6 @@
   </si>
   <si>
     <t>This figure will underestimate the actual number of COVID-19 infections due to people not testing or not being able to report LFD results.</t>
-  </si>
-  <si>
-    <t>COVID-10_cases_countRollingMean</t>
   </si>
   <si>
     <t>This metric shows the average number of cases over the 7 day period ending on the dates shown. 
@@ -196,9 +190,6 @@
 The value shown on a given date is the total of the reported new cases in the 7 days up to and including that date divided by 7.</t>
   </si>
   <si>
-    <t>COVID-10_cases_rateRolling7Day</t>
-  </si>
-  <si>
     <t>This metric shows the rate per 100,000 people of reported new cases in the 7-day period ending on the dates shown. 
 New cases are reported by specimen date - the date the first sample that identified the infection was taken from an individual.</t>
   </si>
@@ -213,9 +204,6 @@
   </si>
   <si>
     <t>Deaths</t>
-  </si>
-  <si>
-    <t>COVID-19_headline_ONSdeaths_7DayTotal</t>
   </si>
   <si>
     <t xml:space="preserve">COVID-19 deaths are an indicator of the scale and severity of current COVID-19 infection levels in the community. </t>
@@ -543,18 +531,12 @@
 This metric is calculated as the difference between (the total of the daily number of beds occupied in the 7 days up to and including the most recent date, divided by 7), and (the the total of the daily number of beds occupied in the previous 7 days , divided by 7), divided by (the total of the daily number of beds occupied in the previous 7 days , divided by 7) </t>
   </si>
   <si>
-    <t>COVID-19_healthcare_admissionsByDay</t>
-  </si>
-  <si>
     <t>This metric shows the daily count of confirmed COVID-19 patients admitted to hospital</t>
   </si>
   <si>
     <t>This data includes people admitted to hospital who tested positive for COVID-19 in the 14 days before their admission and during their stay. Hospital inpatients who are diagnosed with COVID-19 after admission are reported as being admitted on the day before their diagnosis.
 Admissions figures include people admitted to NHS acute hospitals and mental health and learning disability (MHLD) trusts
 Updates are published by NHS England on a Wednesday, and contain data up to the previous Friday.</t>
-  </si>
-  <si>
-    <t>COVID-19_healthcare_admissionsRollingMean</t>
   </si>
   <si>
     <t>This metric shows the average count of admissions with confirmed COVID-19 over the 7 days up to and including the date shown</t>
@@ -683,9 +665,6 @@
     <t>Vaccinations</t>
   </si>
   <si>
-    <t>COVID-19-headline_vaccines_spring23Total</t>
-  </si>
-  <si>
     <t>The COVID-19 vaccine has been shown to be effective in preventing COVID-19 infections and reducing the transmission of the virus.</t>
   </si>
   <si>
@@ -704,9 +683,6 @@
 People who are eligible for an spring booster vaccination but are less than 75 years old (e.g. immunocompromised individuals) are not included in the count.</t>
   </si>
   <si>
-    <t>COVID-19-headline_vaccines_spring23Uptake</t>
-  </si>
-  <si>
     <t>Vaccinations carried out in England are reported in the National Immunisation Management Service (NIMS). This is the system of record for the vaccination programme in England, including both hospital hubs and local vaccination services. Data are extracted at midnight on the date of report.
 Geographic locations of vaccinations are based on where the people who were vaccinated live, and not where the vaccination was given. Vaccinations to England residents that were given outside of England are included if they have been recorded in NIMS. Only people who have an NHS number and are currently alive are included. Age is defined as a person's age at the time the data were extracted.
 This metric shows the percentage uptake of spring booster 2023 vaccinations, and is calculated as the total number of spring booster 2023 vaccinations given to people aged 75 years and over, divided by the number of people who are currently aged 75 years and over.</t>
@@ -779,41 +755,11 @@
     <t>Influenza</t>
   </si>
   <si>
-    <t>Not available during summer reporting period</t>
-  </si>
-  <si>
     <t>Seasonal influenza occurs every year and is a key driver for winter pressure on the NHS. The impact of influenza on the NHS depends on several factors: which strains of the virus are circulating and who is most likely to be affected, how effectve the annual vaccine is, how many people are immunised, and winter temperatures. 
 Understanding rates and patterns of hospital admissions can help to inform planning around hospital pressures including beds and staffing.</t>
   </si>
   <si>
-    <t>This metric shows the rate per 100,000 people of the total number of people with confirmed influenza admitted to hospital in the last 7 days.</t>
-  </si>
-  <si>
-    <t>Count of laboratory-confirmed influenza cases admitted to hospital in the last 7 days</t>
-  </si>
-  <si>
-    <t>Updates from SARI Watch are published in the UKHSA National Influenza and COVID-19 Surveillance Report on a Friday (weekly during influenza season and fortnightly in the summer months), and contains data up to the previous Sunday.
-This metric shows the rate per 100,000 people in the NHS trust catchment population who were admitted to hospital with laboratory-confirmed influenza in the last 7 days.  It is calculated by counting the number of influenza-related admissions in the latest 7 days, dividing by the catchment population of the NHS trust and then multiplying by 100,000.</t>
-  </si>
-  <si>
     <t>Hospital provider trusts do not have geographically defined boundaries for their client population nor do they have all encompassing lists of registered patients. OHID has adopted a proportionate flow method to calculate catchment populations.  Using this method, Hospital Episode Statistics (HES APC) data was used to count the number of patients admitted to hospital from every small geographical area in England (based on middle super output area (MSOSA), which are standard geographies of 7,200 people). For each MSOA, the number of patients admitted to each hospital trust was calculated as a proportion of all patients from that MSOA admitted to hospital. this proportion was then applied to the resident population of each MSOA and the resulting population counts added to give an overall hospital catchment population. The catchment year applies to the year of mid-year population estimates used to calculate the population.</t>
-  </si>
-  <si>
-    <t>This metric shows the change in the rate per 100,000 people of the total number of people with confirmed influenza admitted to hospital in the last 7 days compared to the previous 7 days.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Change in the count of  laboratory-confirmed influenza cases admitted to hospital in the last 7 days compared with the previous 7 days. </t>
-  </si>
-  <si>
-    <t>Updates from SARI Watch are published in the UKHSA National Influenza and COVID-19 Surveillance Report on a Friday (weekly during influenza season and fortnightly in the summer months), and contains data up to the previous Sunday.
-This metric shows the change in rate per 100,000 people in the NHS trust catchment population who were admitted to hospital with laboratory-confirmed influenza in the last 7 days.  It is calculated by subtracting the rate per 100,000 people in the 7 days prior to the last 7 days from the rate people 100,000 people in the last 7 days.  The rate is calculated by counting the number of influenza-related admissions in the 7 day period, dividing by the catchment population of the NHS trust and then multiplying by 100,000.</t>
-  </si>
-  <si>
-    <t>This metric shows the percentage change in the rate per 100,000 people of the total number of people with confirmed influenza admitted to hospital in the last 7 days compared to the previous 7 days.</t>
-  </si>
-  <si>
-    <t>Updates from SARI Watch are published in the UKHSA National Influenza and COVID-19 Surveillance Report on a Friday (weekly during influenza season and fortnightly in the summer months), and contains data up to the previous Sunday.
-This metric shows the percentage change in rate per 100,000 people in the NHS trust catchment population who were admitted to hospital with laboratory-confirmed influenza in the last 7 days.  It is calculated by subtracting the rate per 100,000 people in the 7 days prior to the last 7 days from the rate people 100,000 people in the last 7 days, then dividing by the rate per 100,000 people in the 7 days prior to the last 7 days.  The rate is calculated by counting the number of influenza-related admissions in the 7 day period, dividing by the catchment population of the NHS trust and then multiplying by 100,000.</t>
   </si>
   <si>
     <t>influenza_headline_ICUHDUadmissionRateLatest</t>
@@ -850,16 +796,6 @@
   <si>
     <t>Updates from SARI Watch are published in the UKHSA National Influenza and COVID-19 Surveillance Report on a Friday (weekly during influenza season and fortnightly in the summer months), and contains data up to the previous Sunday.
 This metric shows the percentage change in rate per 100,000 people in the NHS trust catchment population who were admitted to ICU or HDU with laboratory-confirmed influenza in the last 7 days.  It is calculated by subtracting the rate per 100,000 people in the 7 days prior to the last 7 days from the rate people 100,000 people in the last 7 days, then dividing by the rate per 100,000 people in the 7 days prior to the last 7 days.  The rate is calculated by counting the number of influenza-related admissions to ICU or HDU in the 7 day period, dividing by the catchment population of the NHS trust and then multiplying by 100,000.</t>
-  </si>
-  <si>
-    <t>This metric shows the weekly rate per 100,000 people of the total number of people with confirmed influenza admitted to hospital in the 7 days up to and including the date shown.</t>
-  </si>
-  <si>
-    <t>Count of laboratory-confirmed influenza cases admitted to hospital in the previous 7 days</t>
-  </si>
-  <si>
-    <t>Updates from SARI Watch are published in the UKHSA National Influenza and COVID-19 Surveillance Report on a Friday (weekly during influenza season and fortnightly in the summer months), and contains data up to the previous Sunday.
-This metric shows the weekly rate per 100,000 people in the NHS trust catchment population who were admitted to hospital with laboratory-confirmed influenza in the previous 7 days.  It is calculated by counting the number of influenza-related admissions in the 7 days up to and including the date shown, dividing by the catchment population of the NHS trust and then multiplying by 100,000.</t>
   </si>
   <si>
     <t>influenza_healthcare_ICUHDUadmissionRateByWeek</t>
@@ -938,26 +874,6 @@
 This metric shows the rate per 100,000 people in the NHS trust catchment population who were admitted to hospital with laboratory-confirmed RSV in the 7 days up to and including the date shown.  It is calculated by counting the number of RSV-related admissions in the 7 days up to and including the date shown, dividing by the catchment population of the NHS trust and then multiplying by 100,000.</t>
   </si>
   <si>
-    <t>This metric shows the number of people with confirmed RSV admitted to hospital in the 7 days up to and including the date shown</t>
-  </si>
-  <si>
-    <t>Count of laboratory-confirmed RSV cases admitted to hospital in the previous 7 days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Updates from SARI Watch are published in the UKHSA National Influenza and COVID-19 Surveillance Report on a Friday (weekly during influenza season and fortnightly in the summer months), and contains data up to the previous Sunday.
-This metric shows the number of people in the NHS trust catchment population who were admitted to hospital with laboratory-confirmed RSV in the 7 days up to and including the date shown. </t>
-  </si>
-  <si>
-    <t>This metric shows the number of people with confirmed RSV admitted to a hospital intensive care unit (ICU) or high dependency unit (HDU) in the 7 days up to and including the date shown</t>
-  </si>
-  <si>
-    <t>Count of laboratory-confirmed RSV cases admitted to ICU or HDU in the previous 7 days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Updates from SARI Watch are published in the UKHSA National Influenza and COVID-19 Surveillance Report on a Friday (weekly during influenza season and fortnightly in the summer months), and contains data up to the previous Sunday.
-This metric shows the number of people in the NHS trust catchment population who were admitted to ICU or HDU with laboratory-confirmed RSV in the 7 days up to and including the date shown. </t>
-  </si>
-  <si>
     <t>Adenovirus</t>
   </si>
   <si>
@@ -1133,6 +1049,30 @@
     <t>Testing for RSV is performed using polymerase chain reaction (PCR) tests, which require processing in a laboratory
 Updates from SARI Watch are published in the UKHSA National Influenza and COVID-19 Surveillance Report on a Friday (weekly during influenza season and fortnightly in the summer months), and contains data up to the previous Sunday. 
 Weekly positivity is calculated as the count of number of PCR tests taken in the last 7 days up to and including the date shown which had a positive result, divided by the total number of positiv or negative PCR tests taken in the last 7 days up to and including the date shown.</t>
+  </si>
+  <si>
+    <t>COVID-19_cases_casesByDay</t>
+  </si>
+  <si>
+    <t>COVID-19_cases_countRollingMean</t>
+  </si>
+  <si>
+    <t>COVID-19_cases_rateRollingMean</t>
+  </si>
+  <si>
+    <t>COVID-19_headline_ONSdeaths_7DayTotals</t>
+  </si>
+  <si>
+    <t>COVID-19_healthcare_admissionByDay</t>
+  </si>
+  <si>
+    <t>COVID-19_healthcare_admissionRollingMean</t>
+  </si>
+  <si>
+    <t>COVID-19_headline_vaccines_spring23Total</t>
+  </si>
+  <si>
+    <t>COVID-19_headline_vaccines_spring23Uptake</t>
   </si>
 </sst>
 </file>
@@ -1512,7 +1452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1711,9 +1651,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2061,13 +1998,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E3E244-777F-44C7-8F0C-8F9E73605F19}">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1:I1048576"/>
+      <selection pane="bottomRight" activeCell="A43" sqref="A43:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2075,8 +2012,8 @@
     <col min="1" max="1" width="16.1640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="19.5" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="62.6640625" style="73" customWidth="1"/>
-    <col min="5" max="5" width="106.1640625" style="73" customWidth="1"/>
+    <col min="4" max="4" width="62.6640625" style="72" customWidth="1"/>
+    <col min="5" max="5" width="106.1640625" style="72" customWidth="1"/>
     <col min="6" max="6" width="34.6640625" style="6" customWidth="1"/>
     <col min="7" max="7" width="91.6640625" style="6" customWidth="1"/>
     <col min="8" max="8" width="47" style="6" customWidth="1"/>
@@ -2195,22 +2132,22 @@
         <v>9</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>26</v>
+        <v>226</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="304" customHeight="1" x14ac:dyDescent="0.2">
@@ -2221,22 +2158,22 @@
         <v>9</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>31</v>
+        <v>227</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="304" x14ac:dyDescent="0.2">
@@ -2247,22 +2184,22 @@
         <v>9</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>34</v>
+        <v>228</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="237.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2270,22 +2207,22 @@
         <v>8</v>
       </c>
       <c r="B8" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="G8" s="17" t="s">
         <v>38</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>42</v>
       </c>
       <c r="H8" s="18"/>
     </row>
@@ -2294,22 +2231,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C9" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>43</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>47</v>
       </c>
       <c r="H9" s="17"/>
     </row>
@@ -2318,25 +2255,25 @@
         <v>8</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="17" t="s">
-        <v>50</v>
-      </c>
       <c r="H10" s="17" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="202.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2344,22 +2281,22 @@
         <v>8</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H11" s="17"/>
     </row>
@@ -2368,22 +2305,22 @@
         <v>8</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F12" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>54</v>
-      </c>
-      <c r="G12" s="25" t="s">
-        <v>58</v>
       </c>
       <c r="H12" s="25"/>
     </row>
@@ -2392,22 +2329,22 @@
         <v>8</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H13" s="17"/>
     </row>
@@ -2416,22 +2353,22 @@
         <v>8</v>
       </c>
       <c r="B14" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="G14" s="30" t="s">
         <v>64</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="G14" s="30" t="s">
-        <v>68</v>
       </c>
       <c r="H14" s="32"/>
     </row>
@@ -2440,22 +2377,22 @@
         <v>8</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G15" s="35" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H15" s="34"/>
     </row>
@@ -2464,25 +2401,25 @@
         <v>8</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F16" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="36" t="s">
-        <v>75</v>
-      </c>
       <c r="H16" s="37" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="176" x14ac:dyDescent="0.2">
@@ -2490,22 +2427,22 @@
         <v>8</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G17" s="39" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H17" s="40"/>
     </row>
@@ -2514,22 +2451,22 @@
         <v>8</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F18" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="39" t="s">
         <v>78</v>
-      </c>
-      <c r="G18" s="39" t="s">
-        <v>82</v>
       </c>
       <c r="H18" s="40"/>
     </row>
@@ -2538,25 +2475,25 @@
         <v>8</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G19" s="39" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H19" s="41" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="156.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2564,22 +2501,22 @@
         <v>8</v>
       </c>
       <c r="B20" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>67</v>
-      </c>
       <c r="G20" s="43" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H20" s="44"/>
     </row>
@@ -2588,22 +2525,22 @@
         <v>8</v>
       </c>
       <c r="B21" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="F21" s="26" t="s">
-        <v>67</v>
-      </c>
       <c r="G21" s="45" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H21" s="46"/>
     </row>
@@ -2612,22 +2549,22 @@
         <v>8</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C22" s="42" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D22" s="43" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G22" s="48" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H22" s="46"/>
     </row>
@@ -2636,25 +2573,25 @@
         <v>8</v>
       </c>
       <c r="B23" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="51" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="G23" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="H23" s="55" t="s">
         <v>96</v>
-      </c>
-      <c r="C23" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="E23" s="53" t="s">
-        <v>99</v>
-      </c>
-      <c r="F23" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" s="54" t="s">
-        <v>101</v>
-      </c>
-      <c r="H23" s="55" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="128" x14ac:dyDescent="0.2">
@@ -2662,25 +2599,25 @@
         <v>8</v>
       </c>
       <c r="B24" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="H24" s="57" t="s">
         <v>96</v>
-      </c>
-      <c r="C24" s="51" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="E24" s="56" t="s">
-        <v>104</v>
-      </c>
-      <c r="F24" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="G24" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="H24" s="57" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="160" x14ac:dyDescent="0.2">
@@ -2688,25 +2625,25 @@
         <v>8</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D25" s="52" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E25" s="58" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F25" s="49" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G25" s="54" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="H25" s="57" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="160" x14ac:dyDescent="0.2">
@@ -2714,25 +2651,25 @@
         <v>8</v>
       </c>
       <c r="B26" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="H26" s="57" t="s">
         <v>96</v>
-      </c>
-      <c r="C26" s="51" t="s">
-        <v>111</v>
-      </c>
-      <c r="D26" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="E26" s="59" t="s">
-        <v>112</v>
-      </c>
-      <c r="F26" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="G26" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="H26" s="57" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="112" x14ac:dyDescent="0.2">
@@ -2740,25 +2677,25 @@
         <v>8</v>
       </c>
       <c r="B27" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="53" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="G27" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="H27" s="57" t="s">
         <v>96</v>
-      </c>
-      <c r="C27" s="51" t="s">
-        <v>115</v>
-      </c>
-      <c r="D27" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="E27" s="53" t="s">
-        <v>116</v>
-      </c>
-      <c r="F27" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="G27" s="54" t="s">
-        <v>118</v>
-      </c>
-      <c r="H27" s="57" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="144" x14ac:dyDescent="0.2">
@@ -2766,25 +2703,25 @@
         <v>8</v>
       </c>
       <c r="B28" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="G28" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="H28" s="57" t="s">
         <v>96</v>
-      </c>
-      <c r="C28" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="D28" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="E28" s="59" t="s">
-        <v>120</v>
-      </c>
-      <c r="F28" s="49" t="s">
-        <v>121</v>
-      </c>
-      <c r="G28" s="54" t="s">
-        <v>122</v>
-      </c>
-      <c r="H28" s="57" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="176" x14ac:dyDescent="0.2">
@@ -2792,25 +2729,25 @@
         <v>8</v>
       </c>
       <c r="B29" s="63" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C29" s="64" t="s">
-        <v>124</v>
+        <v>232</v>
       </c>
       <c r="D29" s="65" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E29" s="66" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F29" s="62" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="G29" s="66" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H29" s="66" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -2818,25 +2755,25 @@
         <v>8</v>
       </c>
       <c r="B30" s="63" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="64" t="s">
+        <v>233</v>
+      </c>
+      <c r="D30" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="F30" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="G30" s="66" t="s">
         <v>123</v>
       </c>
-      <c r="C30" s="64" t="s">
-        <v>130</v>
-      </c>
-      <c r="D30" s="65" t="s">
-        <v>125</v>
-      </c>
-      <c r="E30" s="66" t="s">
-        <v>126</v>
-      </c>
-      <c r="F30" s="62" t="s">
-        <v>127</v>
-      </c>
-      <c r="G30" s="66" t="s">
-        <v>131</v>
-      </c>
       <c r="H30" s="66" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="176" x14ac:dyDescent="0.2">
@@ -2844,25 +2781,25 @@
         <v>8</v>
       </c>
       <c r="B31" s="63" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C31" s="64" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D31" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="E31" s="66" t="s">
         <v>125</v>
       </c>
-      <c r="E31" s="66" t="s">
-        <v>133</v>
-      </c>
       <c r="F31" s="62" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G31" s="66" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="H31" s="66" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -2870,25 +2807,25 @@
         <v>8</v>
       </c>
       <c r="B32" s="63" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C32" s="64" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D32" s="65" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E32" s="66" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="F32" s="62" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="G32" s="66" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="H32" s="66" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="176" x14ac:dyDescent="0.2">
@@ -2896,25 +2833,25 @@
         <v>8</v>
       </c>
       <c r="B33" s="63" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C33" s="64" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D33" s="65" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E33" s="66" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="F33" s="62" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="G33" s="66" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="H33" s="66" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -2922,618 +2859,466 @@
         <v>8</v>
       </c>
       <c r="B34" s="63" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C34" s="64" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D34" s="65" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E34" s="66" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F34" s="62" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="G34" s="66" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="H34" s="66" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A35" s="26" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="67" t="s">
-        <v>150</v>
+        <v>59</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>144</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E35" s="34" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F35" s="47" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="G35" s="35" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="H35" s="34" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A36" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="E36" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="B36" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="67" t="s">
+      <c r="F36" s="47" t="s">
         <v>150</v>
       </c>
-      <c r="D36" s="30" t="s">
+      <c r="G36" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="E36" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="F36" s="47" t="s">
-        <v>157</v>
-      </c>
-      <c r="G36" s="35" t="s">
-        <v>158</v>
-      </c>
       <c r="H36" s="34" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A37" s="26" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C37" s="67" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="F37" s="47" t="s">
         <v>150</v>
       </c>
-      <c r="D37" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="E37" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="F37" s="47" t="s">
-        <v>157</v>
-      </c>
       <c r="G37" s="35" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="H37" s="34" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A38" s="26" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C38" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="E38" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="F38" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="G38" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="H38" s="34" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+      <c r="A39" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="51" t="s">
+        <v>159</v>
+      </c>
+      <c r="D39" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="E39" s="59" t="s">
         <v>161</v>
       </c>
-      <c r="D38" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="E38" s="34" t="s">
+      <c r="F39" s="49" t="s">
         <v>162</v>
       </c>
-      <c r="F38" s="47" t="s">
+      <c r="G39" s="54" t="s">
         <v>163</v>
       </c>
-      <c r="G38" s="35" t="s">
+      <c r="H39" s="57"/>
+    </row>
+    <row r="40" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+      <c r="A40" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="H38" s="34" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="272" x14ac:dyDescent="0.2">
-      <c r="A39" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="B39" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="29" t="s">
+      <c r="D40" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="E40" s="59" t="s">
         <v>165</v>
       </c>
-      <c r="D39" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="E39" s="34" t="s">
+      <c r="F40" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="F39" s="47" t="s">
+      <c r="G40" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="G39" s="35" t="s">
+      <c r="H40" s="57"/>
+    </row>
+    <row r="41" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+      <c r="A41" s="47" t="s">
         <v>168</v>
       </c>
-      <c r="H39" s="34" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="272" x14ac:dyDescent="0.2">
-      <c r="A40" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="B40" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C40" s="29" t="s">
+      <c r="B41" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="D40" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="E40" s="34" t="s">
+      <c r="D41" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="E41" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="F40" s="47" t="s">
-        <v>167</v>
-      </c>
-      <c r="G40" s="35" t="s">
+      <c r="F41" s="47" t="s">
         <v>171</v>
       </c>
-      <c r="H40" s="34" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="272" x14ac:dyDescent="0.2">
-      <c r="A41" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="B41" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" s="67" t="s">
-        <v>150</v>
-      </c>
-      <c r="D41" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="E41" s="34" t="s">
+      <c r="G41" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="F41" s="47" t="s">
+      <c r="H41" s="46"/>
+    </row>
+    <row r="42" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+      <c r="A42" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="G41" s="35" t="s">
+      <c r="D42" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="H41" s="34" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="272" x14ac:dyDescent="0.2">
-      <c r="A42" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="B42" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="29" t="s">
+      <c r="F42" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="D42" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="E42" s="34" t="s">
+      <c r="G42" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="F42" s="47" t="s">
+      <c r="H42" s="46"/>
+    </row>
+    <row r="43" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+      <c r="A43" s="68" t="s">
         <v>177</v>
       </c>
-      <c r="G42" s="35" t="s">
+      <c r="B43" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="69" t="s">
         <v>178</v>
       </c>
-      <c r="H42" s="34" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="160" x14ac:dyDescent="0.2">
-      <c r="A43" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="B43" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C43" s="51" t="s">
+      <c r="D43" s="70" t="s">
         <v>179</v>
       </c>
-      <c r="D43" s="52" t="s">
+      <c r="E43" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="E43" s="59" t="s">
+      <c r="F43" s="49" t="s">
         <v>181</v>
       </c>
-      <c r="F43" s="49" t="s">
+      <c r="G43" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="G43" s="54" t="s">
+      <c r="H43" s="71"/>
+    </row>
+    <row r="44" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+      <c r="A44" s="68" t="s">
+        <v>177</v>
+      </c>
+      <c r="B44" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="69" t="s">
         <v>183</v>
       </c>
-      <c r="H43" s="57"/>
-    </row>
-    <row r="44" spans="1:8" ht="160" x14ac:dyDescent="0.2">
-      <c r="A44" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="B44" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C44" s="51" t="s">
+      <c r="D44" s="70" t="s">
+        <v>179</v>
+      </c>
+      <c r="E44" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="D44" s="52" t="s">
-        <v>180</v>
-      </c>
-      <c r="E44" s="59" t="s">
+      <c r="F44" s="49" t="s">
         <v>185</v>
       </c>
-      <c r="F44" s="49" t="s">
+      <c r="G44" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="G44" s="54" t="s">
+      <c r="H44" s="71"/>
+    </row>
+    <row r="45" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+      <c r="A45" s="68" t="s">
         <v>187</v>
       </c>
-      <c r="H44" s="57"/>
-    </row>
-    <row r="45" spans="1:8" ht="112" x14ac:dyDescent="0.2">
-      <c r="A45" s="47" t="s">
+      <c r="B45" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="69" t="s">
         <v>188</v>
       </c>
-      <c r="B45" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C45" s="29" t="s">
+      <c r="D45" s="70" t="s">
         <v>189</v>
       </c>
-      <c r="D45" s="68" t="s">
-        <v>65</v>
-      </c>
-      <c r="E45" s="34" t="s">
+      <c r="E45" s="59" t="s">
         <v>190</v>
       </c>
-      <c r="F45" s="47" t="s">
+      <c r="F45" s="49" t="s">
         <v>191</v>
       </c>
-      <c r="G45" s="35" t="s">
+      <c r="G45" s="54" t="s">
         <v>192</v>
       </c>
-      <c r="H45" s="46"/>
-    </row>
-    <row r="46" spans="1:8" ht="128" x14ac:dyDescent="0.2">
-      <c r="A46" s="47" t="s">
-        <v>188</v>
-      </c>
-      <c r="B46" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" s="29" t="s">
+      <c r="H45" s="71"/>
+    </row>
+    <row r="46" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+      <c r="A46" s="68" t="s">
+        <v>187</v>
+      </c>
+      <c r="B46" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="69" t="s">
         <v>193</v>
       </c>
-      <c r="D46" s="68" t="s">
-        <v>65</v>
-      </c>
-      <c r="E46" s="34" t="s">
+      <c r="D46" s="70" t="s">
+        <v>189</v>
+      </c>
+      <c r="E46" s="59" t="s">
         <v>194</v>
       </c>
-      <c r="F46" s="47" t="s">
+      <c r="F46" s="49" t="s">
         <v>195</v>
       </c>
-      <c r="G46" s="35" t="s">
+      <c r="G46" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="H46" s="46"/>
-    </row>
-    <row r="47" spans="1:8" ht="96" x14ac:dyDescent="0.2">
-      <c r="A47" s="47" t="s">
-        <v>188</v>
-      </c>
-      <c r="B47" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C47" s="67" t="s">
-        <v>150</v>
-      </c>
-      <c r="D47" s="68" t="s">
-        <v>65</v>
-      </c>
-      <c r="E47" s="46" t="s">
+      <c r="H46" s="71"/>
+    </row>
+    <row r="47" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+      <c r="A47" s="68" t="s">
         <v>197</v>
       </c>
-      <c r="F47" s="47" t="s">
+      <c r="B47" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="69" t="s">
         <v>198</v>
       </c>
-      <c r="G47" s="35" t="s">
+      <c r="D47" s="70" t="s">
         <v>199</v>
       </c>
-      <c r="H47" s="46"/>
-    </row>
-    <row r="48" spans="1:8" ht="96" x14ac:dyDescent="0.2">
-      <c r="A48" s="47" t="s">
-        <v>188</v>
-      </c>
-      <c r="B48" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C48" s="67" t="s">
-        <v>150</v>
-      </c>
-      <c r="D48" s="68" t="s">
-        <v>65</v>
-      </c>
-      <c r="E48" s="46" t="s">
+      <c r="E47" s="59" t="s">
         <v>200</v>
       </c>
-      <c r="F48" s="47" t="s">
+      <c r="F47" s="49" t="s">
         <v>201</v>
       </c>
-      <c r="G48" s="35" t="s">
+      <c r="G47" s="54" t="s">
         <v>202</v>
       </c>
-      <c r="H48" s="46"/>
+      <c r="H47" s="71"/>
+    </row>
+    <row r="48" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+      <c r="A48" s="68" t="s">
+        <v>197</v>
+      </c>
+      <c r="B48" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="69" t="s">
+        <v>203</v>
+      </c>
+      <c r="D48" s="70" t="s">
+        <v>199</v>
+      </c>
+      <c r="E48" s="59" t="s">
+        <v>204</v>
+      </c>
+      <c r="F48" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="G48" s="54" t="s">
+        <v>206</v>
+      </c>
+      <c r="H48" s="71"/>
     </row>
     <row r="49" spans="1:8" ht="160" x14ac:dyDescent="0.2">
-      <c r="A49" s="69" t="s">
-        <v>203</v>
+      <c r="A49" s="68" t="s">
+        <v>207</v>
       </c>
       <c r="B49" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C49" s="70" t="s">
-        <v>204</v>
-      </c>
-      <c r="D49" s="71" t="s">
-        <v>205</v>
+        <v>90</v>
+      </c>
+      <c r="C49" s="69" t="s">
+        <v>208</v>
+      </c>
+      <c r="D49" s="70" t="s">
+        <v>209</v>
       </c>
       <c r="E49" s="59" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="F49" s="49" t="s">
+        <v>211</v>
+      </c>
+      <c r="G49" s="54" t="s">
+        <v>212</v>
+      </c>
+      <c r="H49" s="71"/>
+    </row>
+    <row r="50" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+      <c r="A50" s="68" t="s">
         <v>207</v>
       </c>
-      <c r="G49" s="54" t="s">
-        <v>208</v>
-      </c>
-      <c r="H49" s="72"/>
-    </row>
-    <row r="50" spans="1:8" ht="160" x14ac:dyDescent="0.2">
-      <c r="A50" s="69" t="s">
-        <v>203</v>
-      </c>
       <c r="B50" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C50" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="69" t="s">
+        <v>213</v>
+      </c>
+      <c r="D50" s="70" t="s">
         <v>209</v>
       </c>
-      <c r="D50" s="71" t="s">
-        <v>205</v>
-      </c>
       <c r="E50" s="59" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F50" s="49" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="G50" s="54" t="s">
-        <v>212</v>
-      </c>
-      <c r="H50" s="72"/>
+        <v>216</v>
+      </c>
+      <c r="H50" s="71"/>
     </row>
     <row r="51" spans="1:8" ht="144" x14ac:dyDescent="0.2">
-      <c r="A51" s="69" t="s">
-        <v>213</v>
+      <c r="A51" s="68" t="s">
+        <v>168</v>
       </c>
       <c r="B51" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C51" s="70" t="s">
-        <v>214</v>
-      </c>
-      <c r="D51" s="71" t="s">
-        <v>215</v>
+        <v>90</v>
+      </c>
+      <c r="C51" s="69" t="s">
+        <v>217</v>
+      </c>
+      <c r="D51" s="70" t="s">
+        <v>218</v>
       </c>
       <c r="E51" s="59" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="F51" s="49" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G51" s="54" t="s">
+        <v>221</v>
+      </c>
+      <c r="H51" s="71"/>
+    </row>
+    <row r="52" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+      <c r="A52" s="68" t="s">
+        <v>168</v>
+      </c>
+      <c r="B52" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="69" t="s">
+        <v>222</v>
+      </c>
+      <c r="D52" s="70" t="s">
         <v>218</v>
       </c>
-      <c r="H51" s="72"/>
-    </row>
-    <row r="52" spans="1:8" ht="144" x14ac:dyDescent="0.2">
-      <c r="A52" s="69" t="s">
-        <v>213</v>
-      </c>
-      <c r="B52" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C52" s="70" t="s">
-        <v>219</v>
-      </c>
-      <c r="D52" s="71" t="s">
-        <v>215</v>
-      </c>
       <c r="E52" s="59" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="F52" s="49" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="G52" s="54" t="s">
-        <v>222</v>
-      </c>
-      <c r="H52" s="72"/>
-    </row>
-    <row r="53" spans="1:8" ht="160" x14ac:dyDescent="0.2">
-      <c r="A53" s="69" t="s">
-        <v>223</v>
-      </c>
-      <c r="B53" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C53" s="70" t="s">
-        <v>224</v>
-      </c>
-      <c r="D53" s="71" t="s">
         <v>225</v>
       </c>
-      <c r="E53" s="59" t="s">
-        <v>226</v>
-      </c>
-      <c r="F53" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="G53" s="54" t="s">
-        <v>228</v>
-      </c>
-      <c r="H53" s="72"/>
-    </row>
-    <row r="54" spans="1:8" ht="160" x14ac:dyDescent="0.2">
-      <c r="A54" s="69" t="s">
-        <v>223</v>
-      </c>
-      <c r="B54" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C54" s="70" t="s">
-        <v>229</v>
-      </c>
-      <c r="D54" s="71" t="s">
-        <v>225</v>
-      </c>
-      <c r="E54" s="59" t="s">
-        <v>230</v>
-      </c>
-      <c r="F54" s="49" t="s">
-        <v>231</v>
-      </c>
-      <c r="G54" s="54" t="s">
-        <v>232</v>
-      </c>
-      <c r="H54" s="72"/>
-    </row>
-    <row r="55" spans="1:8" ht="160" x14ac:dyDescent="0.2">
-      <c r="A55" s="69" t="s">
-        <v>233</v>
-      </c>
-      <c r="B55" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C55" s="70" t="s">
-        <v>234</v>
-      </c>
-      <c r="D55" s="71" t="s">
-        <v>235</v>
-      </c>
-      <c r="E55" s="59" t="s">
-        <v>236</v>
-      </c>
-      <c r="F55" s="49" t="s">
-        <v>237</v>
-      </c>
-      <c r="G55" s="54" t="s">
-        <v>238</v>
-      </c>
-      <c r="H55" s="72"/>
-    </row>
-    <row r="56" spans="1:8" ht="160" x14ac:dyDescent="0.2">
-      <c r="A56" s="69" t="s">
-        <v>233</v>
-      </c>
-      <c r="B56" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C56" s="70" t="s">
-        <v>239</v>
-      </c>
-      <c r="D56" s="71" t="s">
-        <v>235</v>
-      </c>
-      <c r="E56" s="59" t="s">
-        <v>240</v>
-      </c>
-      <c r="F56" s="49" t="s">
-        <v>241</v>
-      </c>
-      <c r="G56" s="54" t="s">
-        <v>242</v>
-      </c>
-      <c r="H56" s="72"/>
-    </row>
-    <row r="57" spans="1:8" ht="144" x14ac:dyDescent="0.2">
-      <c r="A57" s="69" t="s">
-        <v>188</v>
-      </c>
-      <c r="B57" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C57" s="70" t="s">
-        <v>243</v>
-      </c>
-      <c r="D57" s="71" t="s">
-        <v>244</v>
-      </c>
-      <c r="E57" s="59" t="s">
-        <v>245</v>
-      </c>
-      <c r="F57" s="49" t="s">
-        <v>246</v>
-      </c>
-      <c r="G57" s="54" t="s">
-        <v>247</v>
-      </c>
-      <c r="H57" s="72"/>
-    </row>
-    <row r="58" spans="1:8" ht="144" x14ac:dyDescent="0.2">
-      <c r="A58" s="69" t="s">
-        <v>188</v>
-      </c>
-      <c r="B58" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C58" s="70" t="s">
-        <v>248</v>
-      </c>
-      <c r="D58" s="71" t="s">
-        <v>244</v>
-      </c>
-      <c r="E58" s="59" t="s">
-        <v>249</v>
-      </c>
-      <c r="F58" s="49" t="s">
-        <v>250</v>
-      </c>
-      <c r="G58" s="54" t="s">
-        <v>251</v>
-      </c>
-      <c r="H58" s="72"/>
+      <c r="H52" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>